<commit_message>
Yesterday forgot to push
</commit_message>
<xml_diff>
--- a/Luke Excel Data Analysis/Excel_Data_Analytics_Course-main Luke Youtube/2_Formulas_Functions/1_Formulas_Intro.xlsx
+++ b/Luke Excel Data Analysis/Excel_Data_Analytics_Course-main Luke Youtube/2_Formulas_Functions/1_Formulas_Intro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EXCEL\Luke Excel Data Analysis\Excel_Data_Analytics_Course-main Luke Youtube\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FD1D54-5E70-445F-B720-413AD7C92D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CC40B0-FE68-4659-BBEA-5012DE2A3A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44460" yWindow="-18890" windowWidth="32220" windowHeight="13370" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -414,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -487,6 +476,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,25 +814,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A41B6C-80F1-4D7E-AD46-00EDEBFEC87C}">
   <dimension ref="B1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.9453125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" style="4" customWidth="1"/>
     <col min="7" max="13" width="9" style="4"/>
-    <col min="14" max="14" width="11.26171875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.26953125" style="4" customWidth="1"/>
     <col min="15" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
@@ -886,7 +876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -899,8 +889,48 @@
       <c r="E3" s="10">
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" s="4">
+        <f>C3</f>
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <f>D3+E3</f>
+        <v>130000</v>
+      </c>
+      <c r="H3" s="30">
+        <f>E3/D3</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I3" s="4">
+        <f>H3*D3+D3</f>
+        <v>130000</v>
+      </c>
+      <c r="J3" s="4" t="b">
+        <f>I3=G3</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="b">
+        <f>E3&gt;D3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="b">
+        <f>C3&lt;=$C$15</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="4" t="b">
+        <f>D3&gt;=$C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="4">
+        <f>L3*M3</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="4" t="b">
+        <f>N3=1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -913,8 +943,48 @@
       <c r="E4" s="10">
         <v>12000</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" s="4">
+        <f t="shared" ref="F4:F12" si="0">C4</f>
+        <v>4</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G12" si="1">D4+E4</f>
+        <v>147000</v>
+      </c>
+      <c r="H4" s="30">
+        <f t="shared" ref="H4:H12" si="2">E4/D4</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I12" si="3">H4*D4+D4</f>
+        <v>147000</v>
+      </c>
+      <c r="J4" s="4" t="b">
+        <f t="shared" ref="J4:J12" si="4">I4=G4</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="b">
+        <f t="shared" ref="K4:K12" si="5">E4&gt;D4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="4" t="b">
+        <f t="shared" ref="L4:L12" si="6">C4&lt;=$C$15</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="4" t="b">
+        <f t="shared" ref="M4:M12" si="7">D4&gt;=$C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4:N12" si="8">L4*M4</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="4" t="b">
+        <f t="shared" ref="O4:O12" si="9">N4=1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -927,8 +997,48 @@
       <c r="E5" s="10">
         <v>5000</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" si="2"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>80000</v>
+      </c>
+      <c r="J5" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O5" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -941,8 +1051,48 @@
       <c r="E6" s="10">
         <v>8000</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>118000</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="2"/>
+        <v>7.2727272727272724E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>118000</v>
+      </c>
+      <c r="J6" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -955,8 +1105,48 @@
       <c r="E7" s="10">
         <v>11000</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>136000</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" si="2"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>136000</v>
+      </c>
+      <c r="J7" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -969,8 +1159,48 @@
       <c r="E8" s="10">
         <v>7000</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>97000</v>
+      </c>
+      <c r="H8" s="30">
+        <f t="shared" si="2"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>97000</v>
+      </c>
+      <c r="J8" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -983,8 +1213,48 @@
       <c r="E9" s="10">
         <v>15000</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
+        <v>165000</v>
+      </c>
+      <c r="H9" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>165000</v>
+      </c>
+      <c r="J9" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -997,8 +1267,48 @@
       <c r="E10" s="10">
         <v>13000</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
+        <v>143000</v>
+      </c>
+      <c r="H10" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="3"/>
+        <v>143000</v>
+      </c>
+      <c r="J10" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
@@ -1011,8 +1321,48 @@
       <c r="E11" s="10">
         <v>14000</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>154000</v>
+      </c>
+      <c r="H11" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
+        <v>154000</v>
+      </c>
+      <c r="J11" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M11" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
@@ -1025,23 +1375,67 @@
       <c r="E12" s="13">
         <v>9000</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
+        <v>124000</v>
+      </c>
+      <c r="H12" s="30">
+        <f t="shared" si="2"/>
+        <v>7.8260869565217397E-2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="3"/>
+        <v>124000</v>
+      </c>
+      <c r="J12" s="4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="26"/>
-    </row>
-    <row r="16" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C15" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="28">
+        <v>10000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1056,23 +1450,23 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="4" customWidth="1"/>
     <col min="7" max="7" width="9" style="4"/>
     <col min="8" max="9" width="11" style="4" customWidth="1"/>
     <col min="10" max="11" width="9" style="4"/>
-    <col min="12" max="12" width="12.578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:12" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1104,7 +1498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1176,7 +1570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -1212,7 +1606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1248,7 +1642,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1284,7 +1678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -1320,7 +1714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1350,7 +1744,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1774,7 @@
         <v>143000</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
@@ -1410,7 +1804,7 @@
         <v>154000</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
@@ -1453,26 +1847,26 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="4" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="4"/>
     <col min="8" max="8" width="11" style="4" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.26171875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14.26171875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.26953125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" style="4" customWidth="1"/>
     <col min="12" max="13" width="9" style="4"/>
-    <col min="14" max="14" width="19.15625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:14" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:14" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1510,7 +1904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +1948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1598,7 +1992,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -1642,7 +2036,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1686,7 +2080,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1730,7 +2124,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -1774,7 +2168,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1812,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1850,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
@@ -1888,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
@@ -1939,26 +2333,26 @@
       <selection activeCell="B14" sqref="B14:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="4" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="4"/>
     <col min="8" max="9" width="11" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.26171875" style="4" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.26171875" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.15625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.26953125" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" style="4" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="4" customWidth="1"/>
     <col min="13" max="13" width="9" style="4"/>
-    <col min="14" max="14" width="10.41796875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" style="4" customWidth="1"/>
     <col min="15" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:15" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:15" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -2110,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -2164,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -2218,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -2272,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -2326,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -2380,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -2434,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
@@ -2488,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
@@ -2542,12 +2936,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" s="25" t="s">
         <v>48</v>
       </c>
@@ -2555,7 +2949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="27" t="s">
         <v>49</v>
       </c>

</xml_diff>